<commit_message>
db agg after upload
</commit_message>
<xml_diff>
--- a/Interface/extracted_data.xlsx
+++ b/Interface/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -470,106 +470,673 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>Payment from Sze Ho Pok</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>68.27</v>
       </c>
       <c r="E2" t="n">
-        <v>102.38</v>
+        <v>90.56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>To TS Kwong</t>
+          <t>Payment from Wong Pui</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>83.15000000000001</v>
       </c>
       <c r="E3" t="n">
-        <v>96.38</v>
+        <v>173.71</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-03-01</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>To Ho Pok Sze</t>
+          <t>Payment from Wong Pui</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.59</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>79.40000000000001</v>
       </c>
       <c r="E4" t="n">
-        <v>94.79000000000001</v>
+        <v>253.11</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-02-05</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Payment from Sze Ho Pok</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>99.29000000000001</v>
+        <v>244.11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-05</t>
+          <t>2025-03-05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>From CHAK LUNG DRACO TSUI</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>235.11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Transfer to Revolut user</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>29.58</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>205.53</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TO' CHAK LUNG DRACO TSUI</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>2.73</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>202.8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-03-05</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Reference: To Chak Lung Draco T</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
         <v>9</v>
       </c>
-      <c r="E6" t="n">
-        <v>108.29</v>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>208.65</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-03-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Payment from Sze Ho Pok</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5.85</v>
+      </c>
+      <c r="E10" t="n">
+        <v>210.48</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Transfer from Revolut user</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="E11" t="n">
+        <v>201.48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>From: SHUK HEI MOK</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2.77</v>
+      </c>
+      <c r="E12" t="n">
+        <v>192.48</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>To: www cardiff_ac.uk/sport, 029 2087 4675</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>9</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>92.48</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>68.68000000000001</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-03-11</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>To Pui Chi Angie Wong</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>23.8</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>66.76000000000001</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>To Yin Tong Lee</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
+        <v>57.76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>To TS Kwong</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>9</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>48.76</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-03-14</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>39.76</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-03-18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>9</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>26.89</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>2.87</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>29.66</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-03-21</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>To TS Kwong</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>29.66</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>31.86</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-03-22</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Apple Pay Top-Up by *1 573</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>9</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2.2</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-03-23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Transfer from Revolut user</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="E23" t="n">
+        <v>52.2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-03-24</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>From: SHUK HEI MOK</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>50</v>
+      </c>
+      <c r="E24" t="n">
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-03-24</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>TO' Ona*hungrypanda Co. London</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>9</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>34.2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-03-26</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Apple Pay Top-Up by *1 573</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>120</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>154.2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-03-26</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>34.2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-03-27</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>22.95</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>24.2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-03-28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Payment from Wong Pui</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" t="n">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-03-30</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>To Neo Opco (uk) Limited</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>9</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>21.25</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>giffgaff</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>9</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Onerway</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-03-31</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Apple Pay Top-Up by *1 573</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>13.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
match dashboard graph and t1 with correct db link
</commit_message>
<xml_diff>
--- a/Interface/extracted_data.xlsx
+++ b/Interface/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="27" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -470,7 +470,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-01-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -482,94 +482,703 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>100</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>102.38</v>
+        <v>19.15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-01-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>To TS Kwong</t>
+          <t>To Nanxi L</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>96.38</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-02-03</t>
+          <t>2025-01-06</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>To Ho Pok Sze</t>
+          <t>Payment from Wong Pui</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1.59</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>94.79000000000001</v>
+        <v>101.15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-02-05</t>
+          <t>2025-01-06</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Payment from Sze Ho Pok</t>
+          <t>To Ho Pok Sze</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>1.59</v>
       </c>
       <c r="D5" t="n">
-        <v>4.5</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>99.29000000000001</v>
+        <v>99.56</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-02-05</t>
+          <t>2025-01-06</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>To Korean Cultural Centre UK No.6</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>49.56</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-01-10</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>To Chak Lung Draco T</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>10</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>39.56</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-01-11</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Onerway</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>20.91</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>18.65</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Payment from Wong Pui</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
+        <v>50</v>
+      </c>
+      <c r="E9" t="n">
+        <v>68.65000000000001</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>To Ho Pok Sze</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>12.69</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>55.96</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>To TS Kwong</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>9.25</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>46.71</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Payment from Kw</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>20.15</v>
+      </c>
+      <c r="E12" t="n">
+        <v>48.59</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-01-13</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>From SHUK HE-I MOK</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>40.3</v>
+      </c>
+      <c r="E13" t="n">
+        <v>50.47</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2025-01-15</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>35.48</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Onerway</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>22.21</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13.27</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>From SHUK HE-I MOK</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>20.15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>33.42</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Payment from Kw</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>73.72</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2025-01-17</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Payment from Sze Ho Pok</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>93.87</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2025-01-18</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>To TS Kwong</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>13</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>80.87</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-01-19</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Palace Hair Limit</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>10</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>70.87</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-01-20</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>To Pui Chi Angie Wong</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>50</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>20.87</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-01-22</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Payment from Wong Pui</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>72.77</v>
+      </c>
+      <c r="E22" t="n">
+        <v>30.87</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>25.88</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>9</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-01-23</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>9</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>7.88</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2025-01-27</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Payment from Wong Pui</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>9</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2025-01-28</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>giffgaff</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>10</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2025-01-28</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Payment from Sze Ho Pok</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>75.65000000000001</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-01-28</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>To Ho Pok Sze</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>13.76</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>61.89</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-01-29</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Jingxingexp</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>59.01</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2.88</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-01-30</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
           <t>From CHAK LUNG DRACO TSUI</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1.88</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2025-01-30</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Payment from Sze Ho Pok</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>6.38</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2025-01-30</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Payment from Wong Pui</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>20.38</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
         <v>9</v>
       </c>
-      <c r="E6" t="n">
-        <v>108.29</v>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2025-01-31</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Www.cardiff.ac.uk</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>9</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2.38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dummy data + link r n bs
</commit_message>
<xml_diff>
--- a/Interface/extracted_data.xlsx
+++ b/Interface/extracted_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,7 +434,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="33" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="10" customWidth="1" min="4" max="4"/>
     <col width="9" customWidth="1" min="5" max="5"/>
@@ -470,558 +470,558 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>Apple Pay Top-Up by *2180</t>
         </is>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>43.29</v>
       </c>
       <c r="E2" t="n">
-        <v>19.15</v>
+        <v>56.54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2025-01-01</t>
+          <t>2025-04-01</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>To Nanxi L</t>
+          <t>Apple Pay Top-Up by *1 573</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>1.15</v>
+        <v>70.54000000000001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>101.15</v>
+        <v>61.54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-04-03</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>To Ho Pok Sze</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1.59</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>99.56</v>
+        <v>52.54</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-04-04</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>To Korean Cultural Centre UK No.6</t>
+          <t>Sainsbury's</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>50</v>
+        <v>3.75</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>49.56</v>
+        <v>48.79</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2025-01-10</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>To Chak Lung Draco T</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>39.56</v>
+        <v>39.79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2025-01-11</t>
+          <t>2025-04-05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>TO' Ona*hungrypanda Co. London</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>20.91</v>
+        <v>9</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>18.65</v>
+        <v>30.79</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-04-06</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>To Ching Yin Siu</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>10.15</v>
       </c>
       <c r="D9" t="n">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>68.65000000000001</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-04-11</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>To Ho Pok Sze</t>
+          <t>Apple Pay Top-Up by *1 573</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>12.69</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="E10" t="n">
-        <v>55.96</v>
+        <v>50.64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>To TS Kwong</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>9.25</v>
+        <v>9</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>46.71</v>
+        <v>41.64</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Payment from Kw</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D12" t="n">
-        <v>20.15</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>48.59</v>
+        <v>32.64</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>From SHUK HE-I MOK</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D13" t="n">
-        <v>40.3</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>50.47</v>
+        <v>23.64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2025-01-15</t>
+          <t>2025-04-12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TO' Paypal *apple.com/bill, 35314369001</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>14.99</v>
+        <v>9</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>35.48</v>
+        <v>14.64</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2025-01-16</t>
+          <t>2025-04-14</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>To: Ona*hungrypanda Co. London</t>
+          <t>Apple Pay Top-Up by *2180</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>22.21</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="E15" t="n">
-        <v>13.27</v>
+        <v>64.64</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-01-17</t>
+          <t>2025-04-15</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>From SHUK HE-I MOK</t>
+          <t>Onerway</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>31.26</v>
       </c>
       <c r="D16" t="n">
-        <v>20.15</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>33.42</v>
+        <v>33.38</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2025-01-17</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Payment from Kw</t>
+          <t>Sainsbury's</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>3.69</v>
       </c>
       <c r="D17" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>73.72</v>
+        <v>29.69</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2025-01-17</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Payment from Sze Ho Pok</t>
+          <t>KFC</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>5.97</v>
       </c>
       <c r="D18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>93.87</v>
+        <v>23.72</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2025-01-18</t>
+          <t>2025-04-17</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>To TS Kwong</t>
+          <t>Www.cardiff.ac.uk</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>80.87</v>
+        <v>14.72</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2025-01-19</t>
+          <t>2025-04-21</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TO' Sumup *palace Hair Limit, London</t>
+          <t>Apple Pay Top-Up by *2180</t>
         </is>
       </c>
       <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
         <v>10</v>
       </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
       <c r="E20" t="n">
-        <v>70.87</v>
+        <v>24.72</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2025-01-20</t>
+          <t>2025-04-21</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>To Pui Chi Angie Wong</t>
+          <t>To Chung Ho Ling</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>50</v>
+        <v>5.29</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>20.87</v>
+        <v>19.43</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2025-01-22</t>
+          <t>2025-04-22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>Apple Pay Top-Up by *2180</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>72.77</v>
+        <v>9.19</v>
       </c>
       <c r="E22" t="n">
-        <v>30.87</v>
+        <v>28.62</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
+          <t>2025-04-23</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>TO' Paypal *apple.com/bill, 35314369001</t>
+          <t>Onerway</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>4.99</v>
+        <v>28.62</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>25.88</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
+          <t>2025-04-24</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>TO' www 029 2087 4675</t>
+          <t>From Ona*hungrypanda Co, London</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>4.17</v>
       </c>
       <c r="E24" t="n">
-        <v>6.88</v>
+        <v>4.17</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2025-01-23</t>
+          <t>2025-04-24</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>TO' www 029 2087 4675</t>
+          <t>Apple Pay Top-Up by *1 573</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="E25" t="n">
-        <v>7.88</v>
+        <v>74.17</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2025-01-27</t>
+          <t>2025-04-24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Payment from Wong Pui</t>
+          <t>Reference: To Shuk Hei M</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>14.9</v>
       </c>
       <c r="D26" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>2.88</v>
+        <v>59.27</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2025-01-28</t>
+          <t>2025-04-24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>To: Giffgaff, London</t>
+          <t>To TS Kwong</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>10</v>
+        <v>51.86</v>
       </c>
       <c r="D27" t="n">
         <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>2.88</v>
+        <v>7.41</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2025-01-28</t>
+          <t>2025-04-24</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Payment from Sze Ho Pok</t>
+          <t>Payment from Kw</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1031,154 +1031,28 @@
         <v>4.5</v>
       </c>
       <c r="E28" t="n">
-        <v>75.65000000000001</v>
+        <v>1.91</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2025-01-28</t>
+          <t>2025-04-27</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>To Ho Pok Sze</t>
+          <t>giffgaff</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>13.76</v>
+        <v>10</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>61.89</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2025-01-29</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>To: Jingxingexp, Cardiff</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>59.01</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>2.88</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>2025-01-30</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>From CHAK LUNG DRACO TSUI</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" t="n">
-        <v>1.88</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>2025-01-30</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Payment from Sze Ho Pok</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>6.38</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>2025-01-30</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Payment from Wong Pui</t>
-        </is>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>20.38</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>2025-01-31</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>TO' www cardiff_ac.uk/sport, 029 2087 4675</t>
-        </is>
-      </c>
-      <c r="C34" t="n">
-        <v>9</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0</v>
-      </c>
-      <c r="E34" t="n">
-        <v>1.38</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>2025-01-31</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>To: www cardiff_ac.uk/sport, 029 2087 4675</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>9</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>2.38</v>
+        <v>1.91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>